<commit_message>
Polish details of generation
</commit_message>
<xml_diff>
--- a/src/test/resources/ExampleWithSheetsByHand.xlsx
+++ b/src/test/resources/ExampleWithSheetsByHand.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Constructors" sheetId="1" r:id="rId1"/>
@@ -46,36 +46,18 @@
     <t>getM1FloatResult</t>
   </si>
   <si>
-    <t>getM1FloatX</t>
-  </si>
-  <si>
     <t>getM1DoubleResult</t>
   </si>
   <si>
-    <t>getM1DoubleX</t>
-  </si>
-  <si>
     <t>getM1BooleanResult</t>
   </si>
   <si>
-    <t>getM1BooleanX</t>
-  </si>
-  <si>
     <t>getM1StringResult</t>
   </si>
   <si>
-    <t>getM1StringX</t>
-  </si>
-  <si>
     <t>getM1IntIntResult</t>
   </si>
   <si>
-    <t>getM1IntIntX</t>
-  </si>
-  <si>
-    <t>getM1IntIntY</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
@@ -88,10 +70,28 @@
     <t>"x"</t>
   </si>
   <si>
-    <t>getM1IntX</t>
-  </si>
-  <si>
     <t>getM1Result</t>
+  </si>
+  <si>
+    <t>getM1IntParameter0</t>
+  </si>
+  <si>
+    <t>getM1FloatParameter0</t>
+  </si>
+  <si>
+    <t>getM1DoubleParameter0</t>
+  </si>
+  <si>
+    <t>getM1BooleanParameter0</t>
+  </si>
+  <si>
+    <t>getM1StringParameter0</t>
+  </si>
+  <si>
+    <t>getM1IntIntParameter0</t>
+  </si>
+  <si>
+    <t>getM1IntIntParameter1</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -503,7 +503,7 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -563,7 +563,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -572,7 +574,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -656,7 +658,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -665,7 +669,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -749,16 +753,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -842,7 +848,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -851,10 +859,10 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -863,7 +871,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -872,7 +880,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -881,7 +889,7 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -890,7 +898,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -899,7 +907,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -908,7 +916,7 @@
         <v>-2</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -917,7 +925,7 @@
         <v>-2</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -926,7 +934,7 @@
         <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -938,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,10 +957,10 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -960,7 +968,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -968,7 +976,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -976,7 +984,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -984,7 +992,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -992,7 +1000,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -1000,7 +1008,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -1008,7 +1016,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -1016,7 +1024,7 @@
         <v>110</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1029,19 +1037,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>